<commit_message>
End to end, models training at 53% profit for current season at 27 (65%)
</commit_message>
<xml_diff>
--- a/backend/data/odds/most_hits.xlsx
+++ b/backend/data/odds/most_hits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8403595d4321e36a/Documents/Python/MLB/backend/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8403595d4321e36a/Documents/Python/MLB/backend/data/odds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="884" documentId="11_F25DC773A252ABDACC1048DB2919503A5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A19E2065-40F6-4933-A41D-B822C7C6859C}"/>
+  <xr:revisionPtr revIDLastSave="909" documentId="11_F25DC773A252ABDACC1048DB2919503A5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0C47858-CA7C-4642-922B-05FD71B95EF0}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="260" windowWidth="15690" windowHeight="6910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="0" windowWidth="15690" windowHeight="6910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="37">
   <si>
     <t>visitor</t>
   </si>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E261"/>
+  <dimension ref="A1:E277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="E262" sqref="E262"/>
+    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="G276" sqref="G276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4678,6 +4678,254 @@
         <v>-105</v>
       </c>
     </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A262" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B262" t="s">
+        <v>9</v>
+      </c>
+      <c r="C262" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A263" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B263" t="s">
+        <v>9</v>
+      </c>
+      <c r="C263" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A264" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B264" t="s">
+        <v>11</v>
+      </c>
+      <c r="C264" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A265" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B265" t="s">
+        <v>8</v>
+      </c>
+      <c r="C265" t="s">
+        <v>2</v>
+      </c>
+      <c r="D265">
+        <v>-160</v>
+      </c>
+      <c r="E265">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A266" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B266" t="s">
+        <v>5</v>
+      </c>
+      <c r="C266" t="s">
+        <v>19</v>
+      </c>
+      <c r="D266">
+        <v>-125</v>
+      </c>
+      <c r="E266">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A267" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B267" t="s">
+        <v>21</v>
+      </c>
+      <c r="C267" t="s">
+        <v>18</v>
+      </c>
+      <c r="D267">
+        <v>-120</v>
+      </c>
+      <c r="E267">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A268" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B268" t="s">
+        <v>29</v>
+      </c>
+      <c r="C268" t="s">
+        <v>22</v>
+      </c>
+      <c r="D268">
+        <v>135</v>
+      </c>
+      <c r="E268">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A269" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B269" t="s">
+        <v>32</v>
+      </c>
+      <c r="C269" t="s">
+        <v>25</v>
+      </c>
+      <c r="D269">
+        <v>-110</v>
+      </c>
+      <c r="E269">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A270" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B270" t="s">
+        <v>15</v>
+      </c>
+      <c r="C270" t="s">
+        <v>31</v>
+      </c>
+      <c r="D270">
+        <v>105</v>
+      </c>
+      <c r="E270">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A271" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B271" t="s">
+        <v>28</v>
+      </c>
+      <c r="C271" t="s">
+        <v>14</v>
+      </c>
+      <c r="D271">
+        <v>-125</v>
+      </c>
+      <c r="E271">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A272" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B272" t="s">
+        <v>35</v>
+      </c>
+      <c r="C272" t="s">
+        <v>26</v>
+      </c>
+      <c r="D272">
+        <v>115</v>
+      </c>
+      <c r="E272">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A273" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B273" t="s">
+        <v>10</v>
+      </c>
+      <c r="C273" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A274" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B274" t="s">
+        <v>24</v>
+      </c>
+      <c r="C274" t="s">
+        <v>27</v>
+      </c>
+      <c r="D274">
+        <v>-130</v>
+      </c>
+      <c r="E274">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A275" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B275" t="s">
+        <v>6</v>
+      </c>
+      <c r="C275" t="s">
+        <v>34</v>
+      </c>
+      <c r="D275">
+        <v>-125</v>
+      </c>
+      <c r="E275">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A276" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B276" t="s">
+        <v>33</v>
+      </c>
+      <c r="C276" t="s">
+        <v>3</v>
+      </c>
+      <c r="D276">
+        <v>115</v>
+      </c>
+      <c r="E276">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A277" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B277" t="s">
+        <v>7</v>
+      </c>
+      <c r="C277" t="s">
+        <v>13</v>
+      </c>
+      <c r="D277">
+        <v>105</v>
+      </c>
+      <c r="E277">
+        <v>-140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Regression model implemented. RF: 61, +20.7
</commit_message>
<xml_diff>
--- a/backend/data/odds/most_hits.xlsx
+++ b/backend/data/odds/most_hits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8403595d4321e36a/Documents/Python/MLB/backend/data/odds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="966" documentId="11_F25DC773A252ABDACC1048DB2919503A5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0AD9628-944A-47D3-936E-51CB46F49A48}"/>
+  <xr:revisionPtr revIDLastSave="1277" documentId="11_F25DC773A252ABDACC1048DB2919503A5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99597D2C-CE75-4BE2-8CE9-63777BC20F0E}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="200" windowWidth="15690" windowHeight="6910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="100" windowWidth="15690" windowHeight="6910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="37">
   <si>
     <t>visitor</t>
   </si>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E293"/>
+  <dimension ref="A1:E383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="E292" sqref="E292"/>
+    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
+      <selection activeCell="E384" sqref="E384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5168,6 +5168,1404 @@
         <v>36</v>
       </c>
     </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A294" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B294" t="s">
+        <v>8</v>
+      </c>
+      <c r="C294" t="s">
+        <v>2</v>
+      </c>
+      <c r="D294">
+        <v>-165</v>
+      </c>
+      <c r="E294">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A295" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B295" t="s">
+        <v>5</v>
+      </c>
+      <c r="C295" t="s">
+        <v>19</v>
+      </c>
+      <c r="D295">
+        <v>-120</v>
+      </c>
+      <c r="E295">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A296" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B296" t="s">
+        <v>4</v>
+      </c>
+      <c r="C296" t="s">
+        <v>27</v>
+      </c>
+      <c r="D296">
+        <v>-130</v>
+      </c>
+      <c r="E296">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A297" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B297" t="s">
+        <v>20</v>
+      </c>
+      <c r="C297" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A298" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B298" t="s">
+        <v>15</v>
+      </c>
+      <c r="C298" t="s">
+        <v>31</v>
+      </c>
+      <c r="D298">
+        <v>105</v>
+      </c>
+      <c r="E298">
+        <v>-145</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A299" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B299" t="s">
+        <v>25</v>
+      </c>
+      <c r="C299" t="s">
+        <v>36</v>
+      </c>
+      <c r="D299">
+        <v>120</v>
+      </c>
+      <c r="E299">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A300" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B300" t="s">
+        <v>29</v>
+      </c>
+      <c r="C300" t="s">
+        <v>22</v>
+      </c>
+      <c r="D300">
+        <v>125</v>
+      </c>
+      <c r="E300">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A301" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B301" t="s">
+        <v>34</v>
+      </c>
+      <c r="C301" t="s">
+        <v>14</v>
+      </c>
+      <c r="D301">
+        <v>-125</v>
+      </c>
+      <c r="E301">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A302" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B302" t="s">
+        <v>35</v>
+      </c>
+      <c r="C302" t="s">
+        <v>28</v>
+      </c>
+      <c r="D302">
+        <v>110</v>
+      </c>
+      <c r="E302">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A303" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303" t="s">
+        <v>8</v>
+      </c>
+      <c r="D303">
+        <v>105</v>
+      </c>
+      <c r="E303">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A304" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B304" t="s">
+        <v>2</v>
+      </c>
+      <c r="C304" t="s">
+        <v>9</v>
+      </c>
+      <c r="D304">
+        <v>105</v>
+      </c>
+      <c r="E304">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A305" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B305" t="s">
+        <v>19</v>
+      </c>
+      <c r="C305" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A306" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B306" t="s">
+        <v>20</v>
+      </c>
+      <c r="C306" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A307" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B307" t="s">
+        <v>7</v>
+      </c>
+      <c r="C307" t="s">
+        <v>21</v>
+      </c>
+      <c r="D307">
+        <v>-110</v>
+      </c>
+      <c r="E307">
+        <v>-125</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A308" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B308" t="s">
+        <v>13</v>
+      </c>
+      <c r="C308" t="s">
+        <v>22</v>
+      </c>
+      <c r="D308">
+        <v>-115</v>
+      </c>
+      <c r="E308">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A309" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B309" t="s">
+        <v>33</v>
+      </c>
+      <c r="C309" t="s">
+        <v>31</v>
+      </c>
+      <c r="D309">
+        <v>-135</v>
+      </c>
+      <c r="E309">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A310" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B310" t="s">
+        <v>25</v>
+      </c>
+      <c r="C310" t="s">
+        <v>36</v>
+      </c>
+      <c r="D310">
+        <v>125</v>
+      </c>
+      <c r="E310">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A311" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B311" t="s">
+        <v>34</v>
+      </c>
+      <c r="C311" t="s">
+        <v>14</v>
+      </c>
+      <c r="D311">
+        <v>-150</v>
+      </c>
+      <c r="E311">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A312" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B312" t="s">
+        <v>26</v>
+      </c>
+      <c r="C312" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A313" s="1">
+        <v>44687</v>
+      </c>
+      <c r="B313" t="s">
+        <v>35</v>
+      </c>
+      <c r="C313" t="s">
+        <v>28</v>
+      </c>
+      <c r="D313">
+        <v>-115</v>
+      </c>
+      <c r="E313">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A314" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B314" t="s">
+        <v>6</v>
+      </c>
+      <c r="C314" t="s">
+        <v>8</v>
+      </c>
+      <c r="D314">
+        <v>105</v>
+      </c>
+      <c r="E314">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A315" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B315" t="s">
+        <v>18</v>
+      </c>
+      <c r="C315" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A316" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B316" t="s">
+        <v>4</v>
+      </c>
+      <c r="C316" t="s">
+        <v>27</v>
+      </c>
+      <c r="D316">
+        <v>125</v>
+      </c>
+      <c r="E316">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A317" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B317" t="s">
+        <v>6</v>
+      </c>
+      <c r="C317" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A318" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B318" t="s">
+        <v>7</v>
+      </c>
+      <c r="C318" t="s">
+        <v>21</v>
+      </c>
+      <c r="D318">
+        <v>-110</v>
+      </c>
+      <c r="E318">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A319" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B319" t="s">
+        <v>2</v>
+      </c>
+      <c r="C319" t="s">
+        <v>2</v>
+      </c>
+      <c r="D319">
+        <v>100</v>
+      </c>
+      <c r="E319">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A320" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B320" t="s">
+        <v>19</v>
+      </c>
+      <c r="C320" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A321" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B321" t="s">
+        <v>20</v>
+      </c>
+      <c r="C321" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A322" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B322" t="s">
+        <v>26</v>
+      </c>
+      <c r="C322" t="s">
+        <v>29</v>
+      </c>
+      <c r="D322">
+        <v>-150</v>
+      </c>
+      <c r="E322">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A323" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B323" t="s">
+        <v>34</v>
+      </c>
+      <c r="C323" t="s">
+        <v>14</v>
+      </c>
+      <c r="D323">
+        <v>-150</v>
+      </c>
+      <c r="E323">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A324" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B324" t="s">
+        <v>33</v>
+      </c>
+      <c r="C324" t="s">
+        <v>31</v>
+      </c>
+      <c r="D324">
+        <v>115</v>
+      </c>
+      <c r="E324">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A325" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B325" t="s">
+        <v>25</v>
+      </c>
+      <c r="C325" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A326" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B326" t="s">
+        <v>13</v>
+      </c>
+      <c r="C326" t="s">
+        <v>22</v>
+      </c>
+      <c r="D326">
+        <v>-110</v>
+      </c>
+      <c r="E326">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A327" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B327" t="s">
+        <v>35</v>
+      </c>
+      <c r="C327" t="s">
+        <v>28</v>
+      </c>
+      <c r="D327">
+        <v>115</v>
+      </c>
+      <c r="E327">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A328" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B328" t="s">
+        <v>5</v>
+      </c>
+      <c r="C328" t="s">
+        <v>15</v>
+      </c>
+      <c r="D328">
+        <v>-125</v>
+      </c>
+      <c r="E328">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A329" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B329" t="s">
+        <v>18</v>
+      </c>
+      <c r="C329" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A330" s="1">
+        <v>44688</v>
+      </c>
+      <c r="B330" t="s">
+        <v>25</v>
+      </c>
+      <c r="C330" t="s">
+        <v>36</v>
+      </c>
+      <c r="D330">
+        <v>125</v>
+      </c>
+      <c r="E330">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A331" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B331" t="s">
+        <v>2</v>
+      </c>
+      <c r="C331" t="s">
+        <v>9</v>
+      </c>
+      <c r="D331">
+        <v>-115</v>
+      </c>
+      <c r="E331">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A332" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B332" t="s">
+        <v>6</v>
+      </c>
+      <c r="C332" t="s">
+        <v>8</v>
+      </c>
+      <c r="D332">
+        <v>-120</v>
+      </c>
+      <c r="E332">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A333" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B333" t="s">
+        <v>7</v>
+      </c>
+      <c r="C333" t="s">
+        <v>21</v>
+      </c>
+      <c r="D333">
+        <v>-115</v>
+      </c>
+      <c r="E333">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A334" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B334" t="s">
+        <v>19</v>
+      </c>
+      <c r="C334" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A335" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B335" t="s">
+        <v>20</v>
+      </c>
+      <c r="C335" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A336" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B336" t="s">
+        <v>18</v>
+      </c>
+      <c r="C336" t="s">
+        <v>3</v>
+      </c>
+      <c r="D336">
+        <v>145</v>
+      </c>
+      <c r="E336">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A337" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B337" t="s">
+        <v>13</v>
+      </c>
+      <c r="C337" t="s">
+        <v>22</v>
+      </c>
+      <c r="D337">
+        <v>105</v>
+      </c>
+      <c r="E337">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A338" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B338" t="s">
+        <v>24</v>
+      </c>
+      <c r="C338" t="s">
+        <v>32</v>
+      </c>
+      <c r="D338">
+        <v>-160</v>
+      </c>
+      <c r="E338">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A339" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B339" t="s">
+        <v>25</v>
+      </c>
+      <c r="C339" t="s">
+        <v>36</v>
+      </c>
+      <c r="D339">
+        <v>150</v>
+      </c>
+      <c r="E339">
+        <v>-205</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A340" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B340" t="s">
+        <v>34</v>
+      </c>
+      <c r="C340" t="s">
+        <v>14</v>
+      </c>
+      <c r="D340">
+        <v>-140</v>
+      </c>
+      <c r="E340">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A341" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B341" t="s">
+        <v>26</v>
+      </c>
+      <c r="C341" t="s">
+        <v>29</v>
+      </c>
+      <c r="D341">
+        <v>-135</v>
+      </c>
+      <c r="E341">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A342" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B342" t="s">
+        <v>35</v>
+      </c>
+      <c r="C342" t="s">
+        <v>28</v>
+      </c>
+      <c r="D342">
+        <v>-110</v>
+      </c>
+      <c r="E342">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A343" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B343" t="s">
+        <v>5</v>
+      </c>
+      <c r="C343" t="s">
+        <v>15</v>
+      </c>
+      <c r="D343">
+        <v>-155</v>
+      </c>
+      <c r="E343">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A344" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B344" t="s">
+        <v>24</v>
+      </c>
+      <c r="C344" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A345" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B345" t="s">
+        <v>13</v>
+      </c>
+      <c r="C345" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A346" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B346" t="s">
+        <v>4</v>
+      </c>
+      <c r="C346" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A347" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B347" t="s">
+        <v>18</v>
+      </c>
+      <c r="C347" t="s">
+        <v>6</v>
+      </c>
+      <c r="D347">
+        <v>175</v>
+      </c>
+      <c r="E347">
+        <v>-245</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A348" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B348" t="s">
+        <v>2</v>
+      </c>
+      <c r="C348" t="s">
+        <v>8</v>
+      </c>
+      <c r="D348">
+        <v>125</v>
+      </c>
+      <c r="E348">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A349" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B349" t="s">
+        <v>20</v>
+      </c>
+      <c r="C349" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A350" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B350" t="s">
+        <v>3</v>
+      </c>
+      <c r="C350" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A351" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B351" t="s">
+        <v>19</v>
+      </c>
+      <c r="C351" t="s">
+        <v>21</v>
+      </c>
+      <c r="D351">
+        <v>-165</v>
+      </c>
+      <c r="E351">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A352" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B352" t="s">
+        <v>26</v>
+      </c>
+      <c r="C352" t="s">
+        <v>34</v>
+      </c>
+      <c r="D352">
+        <v>-110</v>
+      </c>
+      <c r="E352">
+        <v>-125</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A353" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B353" t="s">
+        <v>12</v>
+      </c>
+      <c r="C353" t="s">
+        <v>33</v>
+      </c>
+      <c r="D353">
+        <v>-140</v>
+      </c>
+      <c r="E353">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A354" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B354" t="s">
+        <v>35</v>
+      </c>
+      <c r="C354" t="s">
+        <v>15</v>
+      </c>
+      <c r="D354">
+        <v>-115</v>
+      </c>
+      <c r="E354">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A355" s="1">
+        <v>44690</v>
+      </c>
+      <c r="B355" t="s">
+        <v>27</v>
+      </c>
+      <c r="C355" t="s">
+        <v>28</v>
+      </c>
+      <c r="D355">
+        <v>-105</v>
+      </c>
+      <c r="E355">
+        <v>-125</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A356" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B356" t="s">
+        <v>18</v>
+      </c>
+      <c r="C356" t="s">
+        <v>6</v>
+      </c>
+      <c r="D356">
+        <v>165</v>
+      </c>
+      <c r="E356">
+        <v>-225</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A357" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B357" t="s">
+        <v>2</v>
+      </c>
+      <c r="C357" t="s">
+        <v>8</v>
+      </c>
+      <c r="D357">
+        <v>145</v>
+      </c>
+      <c r="E357">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A358" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B358" t="s">
+        <v>3</v>
+      </c>
+      <c r="C358" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A359" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B359" t="s">
+        <v>20</v>
+      </c>
+      <c r="C359" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A360" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B360" t="s">
+        <v>19</v>
+      </c>
+      <c r="C360" t="s">
+        <v>21</v>
+      </c>
+      <c r="D360">
+        <v>-150</v>
+      </c>
+      <c r="E360">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A361" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B361" t="s">
+        <v>34</v>
+      </c>
+      <c r="C361" t="s">
+        <v>26</v>
+      </c>
+      <c r="D361">
+        <v>-105</v>
+      </c>
+      <c r="E361">
+        <v>-130</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A362" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B362" t="s">
+        <v>26</v>
+      </c>
+      <c r="C362" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A363" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B363" t="s">
+        <v>25</v>
+      </c>
+      <c r="C363" t="s">
+        <v>32</v>
+      </c>
+      <c r="D363">
+        <v>-135</v>
+      </c>
+      <c r="E363">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A364" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B364" t="s">
+        <v>14</v>
+      </c>
+      <c r="C364" t="s">
+        <v>29</v>
+      </c>
+      <c r="D364">
+        <v>125</v>
+      </c>
+      <c r="E364">
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A365" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B365" t="s">
+        <v>13</v>
+      </c>
+      <c r="C365" t="s">
+        <v>24</v>
+      </c>
+      <c r="D365">
+        <v>-120</v>
+      </c>
+      <c r="E365">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A366" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B366" t="s">
+        <v>12</v>
+      </c>
+      <c r="C366" t="s">
+        <v>33</v>
+      </c>
+      <c r="D366">
+        <v>-135</v>
+      </c>
+      <c r="E366">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A367" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B367" t="s">
+        <v>35</v>
+      </c>
+      <c r="C367" t="s">
+        <v>15</v>
+      </c>
+      <c r="D367">
+        <v>105</v>
+      </c>
+      <c r="E367">
+        <v>-135</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A368" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B368" t="s">
+        <v>31</v>
+      </c>
+      <c r="C368" t="s">
+        <v>9</v>
+      </c>
+      <c r="D368">
+        <v>-115</v>
+      </c>
+      <c r="E368">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A369" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B369" t="s">
+        <v>27</v>
+      </c>
+      <c r="C369" t="s">
+        <v>28</v>
+      </c>
+      <c r="D369">
+        <v>110</v>
+      </c>
+      <c r="E369">
+        <v>-145</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A370" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B370" t="s">
+        <v>18</v>
+      </c>
+      <c r="C370" t="s">
+        <v>6</v>
+      </c>
+      <c r="D370">
+        <v>150</v>
+      </c>
+      <c r="E370">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A371" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B371" t="s">
+        <v>2</v>
+      </c>
+      <c r="C371" t="s">
+        <v>8</v>
+      </c>
+      <c r="D371">
+        <v>150</v>
+      </c>
+      <c r="E371">
+        <v>-205</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A372" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B372" t="s">
+        <v>20</v>
+      </c>
+      <c r="C372" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A373" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B373" t="s">
+        <v>19</v>
+      </c>
+      <c r="C373" t="s">
+        <v>21</v>
+      </c>
+      <c r="D373">
+        <v>-150</v>
+      </c>
+      <c r="E373">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A374" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B374" t="s">
+        <v>3</v>
+      </c>
+      <c r="C374" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A375" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B375" t="s">
+        <v>4</v>
+      </c>
+      <c r="C375" t="s">
+        <v>5</v>
+      </c>
+      <c r="D375">
+        <v>145</v>
+      </c>
+      <c r="E375">
+        <v>-195</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A376" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B376" t="s">
+        <v>25</v>
+      </c>
+      <c r="C376" t="s">
+        <v>32</v>
+      </c>
+      <c r="D376">
+        <v>-115</v>
+      </c>
+      <c r="E376">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A377" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B377" t="s">
+        <v>12</v>
+      </c>
+      <c r="C377" t="s">
+        <v>33</v>
+      </c>
+      <c r="D377">
+        <v>-115</v>
+      </c>
+      <c r="E377">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A378" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B378" t="s">
+        <v>35</v>
+      </c>
+      <c r="C378" t="s">
+        <v>15</v>
+      </c>
+      <c r="D378">
+        <v>-115</v>
+      </c>
+      <c r="E378">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A379" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B379" t="s">
+        <v>26</v>
+      </c>
+      <c r="C379" t="s">
+        <v>34</v>
+      </c>
+      <c r="D379">
+        <v>-110</v>
+      </c>
+      <c r="E379">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A380" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B380" t="s">
+        <v>14</v>
+      </c>
+      <c r="C380" t="s">
+        <v>29</v>
+      </c>
+      <c r="D380">
+        <v>105</v>
+      </c>
+      <c r="E380">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A381" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B381" t="s">
+        <v>27</v>
+      </c>
+      <c r="C381" t="s">
+        <v>28</v>
+      </c>
+      <c r="D381">
+        <v>-120</v>
+      </c>
+      <c r="E381">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A382" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B382" t="s">
+        <v>31</v>
+      </c>
+      <c r="C382" t="s">
+        <v>9</v>
+      </c>
+      <c r="D382">
+        <v>-110</v>
+      </c>
+      <c r="E382">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A383" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B383" t="s">
+        <v>22</v>
+      </c>
+      <c r="C383" t="s">
+        <v>7</v>
+      </c>
+      <c r="D383">
+        <v>-155</v>
+      </c>
+      <c r="E383">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>